<commit_message>
Initial commit for sensitivity
</commit_message>
<xml_diff>
--- a/micro-benchmark/track.xlsx
+++ b/micro-benchmark/track.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thesis\micro-benchmark\CamBench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sam\master-thesis-of-samkutty\micro-benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908BF651-68D2-433A-B961-E8FCF67A0CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864854EE-1388-4A55-B22E-4595E42C8B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="cambench" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="173">
   <si>
     <t>basic</t>
   </si>
@@ -503,6 +504,60 @@
   </si>
   <si>
     <t>simple</t>
+  </si>
+  <si>
+    <t>contextfield</t>
+  </si>
+  <si>
+    <t>contextflow</t>
+  </si>
+  <si>
+    <t>contextobject</t>
+  </si>
+  <si>
+    <t>contextpath</t>
+  </si>
+  <si>
+    <t>fieldflow</t>
+  </si>
+  <si>
+    <t>fieldobject</t>
+  </si>
+  <si>
+    <t>fieldpath</t>
+  </si>
+  <si>
+    <t>flowobject</t>
+  </si>
+  <si>
+    <t>flowpath</t>
+  </si>
+  <si>
+    <t>inter2context</t>
+  </si>
+  <si>
+    <t>inter2field</t>
+  </si>
+  <si>
+    <t>inter2flow</t>
+  </si>
+  <si>
+    <t>inter2object</t>
+  </si>
+  <si>
+    <t>inter2path</t>
+  </si>
+  <si>
+    <t>objectpath</t>
+  </si>
+  <si>
+    <t>arithmetic</t>
+  </si>
+  <si>
+    <t>interprocedural</t>
+  </si>
+  <si>
+    <t>intraprocedural</t>
   </si>
 </sst>
 </file>
@@ -583,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -970,11 +1025,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1124,6 +1317,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1768,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48299460-FF67-475F-8367-3C54998AD978}">
   <dimension ref="C2:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2977,4 +3227,355 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3703AB-8E7D-42A3-96C7-F31E798E4220}">
+  <dimension ref="B3:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="61"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="61"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="61"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="61"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="60"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="61"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="60"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="61"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="60"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="61"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="61"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="62"/>
+      <c r="C14" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="61"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="62"/>
+      <c r="C15" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="61"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="62"/>
+      <c r="C16" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="61"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="62"/>
+      <c r="C17" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="61"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="62"/>
+      <c r="C18" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="61"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="62"/>
+      <c r="C19" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="61"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="62"/>
+      <c r="C20" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="61"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="62"/>
+      <c r="C21" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="61"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="62"/>
+      <c r="C22" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="61"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="62"/>
+      <c r="C23" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="61"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="62"/>
+      <c r="C24" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="61"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="62"/>
+      <c r="C25" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="61"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="62"/>
+      <c r="C26" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="61"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="62"/>
+      <c r="C27" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="61"/>
+    </row>
+    <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="65"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B13:B27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mixed_sensitives - initial commit
</commit_message>
<xml_diff>
--- a/micro-benchmark/track.xlsx
+++ b/micro-benchmark/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sam\master-thesis-of-samkutty\micro-benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00C2641-981B-49F4-9508-120B4EA397A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98E4A88-7ECE-4A77-B48E-A7B028389C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3234,7 +3234,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3395,7 +3395,7 @@
       <c r="C15" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -3408,7 +3408,7 @@
       <c r="C16" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -3421,7 +3421,7 @@
       <c r="C17" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3434,7 +3434,7 @@
       <c r="C18" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -3447,7 +3447,7 @@
       <c r="C19" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -3460,7 +3460,7 @@
       <c r="C20" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -3473,7 +3473,7 @@
       <c r="C21" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -3551,7 +3551,7 @@
       <c r="C27" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>

</xml_diff>

<commit_message>
Some more programs for sensitivity
</commit_message>
<xml_diff>
--- a/micro-benchmark/track.xlsx
+++ b/micro-benchmark/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sam\master-thesis-of-samkutty\micro-benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98E4A88-7ECE-4A77-B48E-A7B028389C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7C5021-171C-4AE6-9BD4-B0C72A6E2BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3293" yWindow="3293" windowWidth="20531" windowHeight="10722" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="176">
   <si>
     <t>basic</t>
   </si>
@@ -558,6 +558,15 @@
   </si>
   <si>
     <t>intraprocedural</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>len</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3243,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3251,9 +3260,15 @@
       <c r="D4" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="E4" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>175</v>
+      </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
       <c r="J4" s="47"/>

</xml_diff>